<commit_message>
Updated Attendence sheet 01/11/23
</commit_message>
<xml_diff>
--- a/Minutes and Attendance/Attendance Sheet.xlsx
+++ b/Minutes and Attendance/Attendance Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakot\OneDrive\Documents\GitHub\Experimental-Systems-Project\Minutes and Attendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2CCA9E-6E48-406F-91FB-63B46CDFB02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1207649B-621B-41AD-AE35-455357B4C8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B31F345-99C4-4C62-96DF-A9974D1B2469}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t xml:space="preserve">Jason </t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Reason for absence</t>
+  </si>
+  <si>
+    <t>31/11/2023</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -318,10 +321,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F5BC01-B091-424A-9FDC-D946B9AC7A0C}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,9 +663,12 @@
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20"/>
       <c r="B1" s="21">
         <v>45212</v>
@@ -676,8 +688,20 @@
       <c r="G1" s="21">
         <v>45258</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="21">
+        <v>45233</v>
+      </c>
+      <c r="J1" s="21">
+        <v>45237</v>
+      </c>
+      <c r="K1" s="21">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="23" t="s">
         <v>9</v>
@@ -697,8 +721,20 @@
       <c r="G2" s="25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -707,18 +743,26 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="14"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18"/>
       <c r="B4" s="10"/>
       <c r="C4" s="4"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="29"/>
-    </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
@@ -727,18 +771,26 @@
       <c r="D5" s="14"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+    </row>
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19"/>
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="15"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+    </row>
+    <row r="7" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
@@ -747,18 +799,26 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="28"/>
-    </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+    </row>
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19"/>
       <c r="B8" s="13"/>
       <c r="C8" s="7"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+    </row>
+    <row r="9" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
@@ -767,18 +827,26 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="28"/>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="11"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+    </row>
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="12"/>
       <c r="C10" s="2"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="12"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+    </row>
+    <row r="11" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>4</v>
       </c>
@@ -787,18 +855,26 @@
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+    </row>
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="12"/>
       <c r="C12" s="2"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+    </row>
+    <row r="13" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>6</v>
       </c>
@@ -807,18 +883,26 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="14"/>
-      <c r="G13" s="28"/>
-    </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="12"/>
       <c r="C14" s="2"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+    </row>
+    <row r="15" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>5</v>
       </c>
@@ -827,9 +911,13 @@
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="29"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+    </row>
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="12"/>
       <c r="C16" s="2"/>
@@ -837,8 +925,12 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="30"/>
-    </row>
-    <row r="17" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="12"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+    </row>
+    <row r="17" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>7</v>
       </c>
@@ -847,31 +939,39 @@
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="28"/>
-    </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+    </row>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="12"/>
       <c r="C18" s="2"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="26"/>
       <c r="D21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C22" s="31"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="28"/>
       <c r="D22" t="s">
         <v>12</v>
       </c>

</xml_diff>